<commit_message>
Use base64 to encode the Association for Science and Technology logo
</commit_message>
<xml_diff>
--- a/src/main/resources/static/UserTemplate.xlsx
+++ b/src/main/resources/static/UserTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\web\gctaatt\GCTAAttendanceSystem\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FF212D-C539-4481-B4D6-FE1B6A42BDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29531AD1-E845-4BE0-A920-A12FDAF12961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="204" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -445,13 +445,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{6E9C0A1A-C616-4C7C-A019-BA605E9F158C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576 C2" xr:uid="{6E9C0A1A-C616-4C7C-A019-BA605E9F158C}">
       <formula1>"多媒体部,硬件部,软件部"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{E410D9CD-7A00-407D-9E2E-AE96811691ED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576 D2" xr:uid="{E410D9CD-7A00-407D-9E2E-AE96811691ED}">
       <formula1>"5102,5108,5109"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{1A649B50-9BA9-4173-903E-19720DFDB42F}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 F2" xr:uid="{1A649B50-9BA9-4173-903E-19720DFDB42F}">
       <formula1>0</formula1>
       <formula2>99</formula2>
     </dataValidation>

</xml_diff>